<commit_message>
global advancement 70% : - Perimeter = > 100% - First Analysis=> 100% - First clean data= >100% - Selection of the dataset for the project=> 90% - Clean data ( outliers , missing data, duplicate) => 80% - Analysis statistics ( ANOVA, ACP, etc...) => 60%
To do after : 
- Analysis dynamics
- PPT
- Web page => Voilà librairies
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_3\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0ADCDD-686E-400F-A4E2-D783998E24CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E47069-0F79-4B5E-A7A4-F9776C6E9C96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Effectuer des opérations de nettoyage sur des données structurées</t>
+  </si>
+  <si>
+    <t>Commentaire</t>
+  </si>
+  <si>
+    <t>Rajouter des fonctions de nettoyage automatique +</t>
   </si>
 </sst>
 </file>
@@ -157,7 +163,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,8 +212,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -231,19 +243,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -268,17 +267,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -294,15 +282,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -310,6 +329,71 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -322,35 +406,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -367,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -375,16 +431,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -393,39 +460,44 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -712,13 +784,14 @@
   <dimension ref="B2:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="56.81640625" customWidth="1"/>
     <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -727,191 +800,226 @@
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="2:8" ht="39" customHeight="1" thickBot="1">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="12">
+        <v>1</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="F5" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="F6" s="10">
+        <f>AVERAGE(C5:C11,C13:C17,C19:C23)</f>
+        <v>0.78882352941176481</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="12">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="63" customHeight="1">
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12">
+        <v>1</v>
+      </c>
+      <c r="D8" s="17"/>
+    </row>
+    <row r="9" spans="2:8" ht="62" customHeight="1">
+      <c r="B9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="2:8" ht="93.5" customHeight="1">
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.66</v>
+      </c>
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="2:8" ht="82.5" customHeight="1" thickBot="1">
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B12" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="D13" s="19"/>
+    </row>
+    <row r="14" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.8</v>
+      </c>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="12">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="2:8" ht="40.5" customHeight="1">
+      <c r="B16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.4</v>
+      </c>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="17" spans="2:4" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="2:4" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B18" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="23"/>
+      <c r="D18" s="20"/>
+    </row>
+    <row r="19" spans="2:4" ht="40.5" customHeight="1">
+      <c r="B19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="14">
+        <v>1</v>
+      </c>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="2:4" ht="40.5" customHeight="1">
+      <c r="B20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="17"/>
+    </row>
+    <row r="21" spans="2:4" ht="40.5" customHeight="1">
+      <c r="B21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="12">
+        <v>1</v>
+      </c>
+      <c r="D21" s="16"/>
+    </row>
+    <row r="22" spans="2:4" ht="40.5" customHeight="1">
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="12">
+        <v>1</v>
+      </c>
+      <c r="D22" s="17"/>
+    </row>
+    <row r="23" spans="2:4" ht="40.5" customHeight="1" thickBot="1">
+      <c r="B23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="15">
         <v>0</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <f>AVERAGE(C5:C11,C13:C17,C19:C23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="40.5" customHeight="1">
-      <c r="B7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="63" customHeight="1">
-      <c r="B8" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="62" customHeight="1">
-      <c r="B9" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="93.5" customHeight="1">
-      <c r="B10" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="82.5" customHeight="1" thickBot="1">
-      <c r="B11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="9">
-        <v>0</v>
-      </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="2:8" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B12" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="19"/>
-    </row>
-    <row r="13" spans="2:8" ht="40.5" customHeight="1">
-      <c r="B13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="40.5" customHeight="1">
-      <c r="B14" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" ht="40.5" customHeight="1">
-      <c r="B15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="40.5" customHeight="1">
-      <c r="B16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B18" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="21"/>
-    </row>
-    <row r="19" spans="2:3" ht="40.5" customHeight="1">
-      <c r="B19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="40.5" customHeight="1">
-      <c r="B20" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="40.5" customHeight="1">
-      <c r="B21" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="40.5" customHeight="1">
-      <c r="B22" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="40.5" customHeight="1" thickBot="1">
-      <c r="B23" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="40.5" customHeight="1">
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="2:4" ht="40.5" customHeight="1">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:3" ht="27.5" customHeight="1"/>
-    <row r="26" spans="2:3" ht="27.5" customHeight="1"/>
-    <row r="27" spans="2:3" ht="27.5" customHeight="1"/>
-    <row r="28" spans="2:3" ht="27.5" customHeight="1"/>
-    <row r="29" spans="2:3" ht="27.5" customHeight="1"/>
-    <row r="30" spans="2:3" ht="27.5" customHeight="1"/>
-    <row r="31" spans="2:3" ht="27.5" customHeight="1"/>
-    <row r="32" spans="2:3" ht="27.5" customHeight="1"/>
+    <row r="25" spans="2:4" ht="27.5" customHeight="1"/>
+    <row r="26" spans="2:4" ht="27.5" customHeight="1"/>
+    <row r="27" spans="2:4" ht="27.5" customHeight="1"/>
+    <row r="28" spans="2:4" ht="27.5" customHeight="1"/>
+    <row r="29" spans="2:4" ht="27.5" customHeight="1"/>
+    <row r="30" spans="2:4" ht="27.5" customHeight="1"/>
+    <row r="31" spans="2:4" ht="27.5" customHeight="1"/>
+    <row r="32" spans="2:4" ht="27.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B4:C4"/>
   </mergeCells>
+  <conditionalFormatting sqref="C5:C11 C13:C17 C19:C23">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color theme="5"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Global advancement : 90% => Notebook 95% (to do : syntaxe error) => Web Page 50% (voila package install and start to deploy/use) => Présentation 0%
</commit_message>
<xml_diff>
--- a/Ressource/Avancement.xlsx
+++ b/Ressource/Avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenClassroom_projet\Projet_3\Ressource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E47069-0F79-4B5E-A7A4-F9776C6E9C96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234BCC6D-ED74-492C-AC43-87FD91975D0B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Tache à réaliser : </t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>Commentaire</t>
-  </si>
-  <si>
-    <t>Rajouter des fonctions de nettoyage automatique +</t>
   </si>
 </sst>
 </file>
@@ -784,7 +781,7 @@
   <dimension ref="B2:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -836,7 +833,7 @@
       <c r="D6" s="17"/>
       <c r="F6" s="10">
         <f>AVERAGE(C5:C11,C13:C17,C19:C23)</f>
-        <v>0.78882352941176481</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="40.5" customHeight="1">
@@ -846,9 +843,7 @@
       <c r="C7" s="12">
         <v>1</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="2:8" ht="63" customHeight="1">
       <c r="B8" s="6" t="s">
@@ -873,7 +868,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="12">
-        <v>0.66</v>
+        <v>1</v>
       </c>
       <c r="D10" s="17"/>
     </row>
@@ -901,7 +896,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="14">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D13" s="19"/>
     </row>
@@ -910,7 +905,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="12">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D14" s="17"/>
     </row>
@@ -928,7 +923,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="12">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="D16" s="17"/>
     </row>
@@ -937,7 +932,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="13">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="D17" s="21"/>
     </row>
@@ -962,7 +957,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D20" s="17"/>
     </row>
@@ -989,7 +984,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="18"/>
     </row>

</xml_diff>